<commit_message>
la inn siste eksamen og oppdaterte kalender
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H23.xlsx
+++ b/diverse/tidsplan-H23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\met4git\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20390094-41E9-4E56-932D-D8572A61D67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91324B07-468E-4F96-ACE5-41458FE8ADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,13 +138,13 @@
     <t>30.10:  **Oversiktsforelesning: Avansert regresjon og maskinlæring** i Aud A</t>
   </si>
   <si>
-    <t xml:space="preserve"> 06.10: Kontakttime, kursansvarlig tilgjengelig i Aud A</t>
-  </si>
-  <si>
     <t>09.11: Oppgaveseminar 7, Aud A. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
     <t xml:space="preserve"> 02.11: **Oppgaveseminar  6**, Aud A. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06.11: Kontakttime, kursansvarlig tilgjengelig i Aud A</t>
   </si>
 </sst>
 </file>
@@ -471,19 +471,19 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="69.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" customWidth="1"/>
+    <col min="3" max="3" width="69.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>34</v>
       </c>
@@ -511,7 +511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>35</v>
       </c>
@@ -525,7 +525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>36</v>
       </c>
@@ -539,7 +539,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>37</v>
       </c>
@@ -553,7 +553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>38</v>
       </c>
@@ -567,7 +567,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>39</v>
       </c>
@@ -581,7 +581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>40</v>
       </c>
@@ -595,7 +595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>41</v>
       </c>
@@ -609,7 +609,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>42</v>
       </c>
@@ -623,7 +623,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>43</v>
       </c>
@@ -637,7 +637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>44</v>
       </c>
@@ -648,10 +648,10 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>45</v>
       </c>
@@ -659,10 +659,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>